<commit_message>
Added row for release 5.0.1
Added row for release 5.0.1
</commit_message>
<xml_diff>
--- a/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
+++ b/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\bridg-model SVN\trunk\SCC Internal\Graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\bridg-model GitHub\bridg-model\Documents\Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Release</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>NCI's Surveillance, Epidemiology and End Results (SEER) Program Concepts</t>
+  </si>
+  <si>
+    <t>5.0.1</t>
+  </si>
+  <si>
+    <t>Aug. 2017</t>
+  </si>
+  <si>
+    <t>HL7 BRIDG 5.0 DSTU Ballot Comment Resolutions</t>
   </si>
 </sst>
 </file>
@@ -356,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -404,6 +413,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -710,21 +722,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E40"/>
+  <dimension ref="B2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="90" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="92.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
@@ -740,474 +749,488 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C4" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>66</v>
+      <c r="B7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
-        <v>3.2</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="4" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="D13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
+    <row r="17" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="17">
         <v>3.1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="4" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="4" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="9">
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="17">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="17">
         <v>2.1</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="4" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
+      <c r="E32" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="4" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="4" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+      <c r="E35" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C36" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="4" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B27 B32 B35 B37" numberStoredAsText="1"/>
+    <ignoredError sqref="B28 B33 B36 B38" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added row for BRIDG release 5.1
</commit_message>
<xml_diff>
--- a/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
+++ b/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\bridg-model GitHub\bridg-model\Documents\Graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shastak\Documents\Documents\MyDocs\Samvit\Contracts\Attain\BRIDG 5.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23820" windowHeight="9855"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="21984" windowHeight="9972"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>Release</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>HL7 BRIDG 5.0 DSTU Ballot Comment Resolutions</t>
+  </si>
+  <si>
+    <t>Mar. 2018</t>
+  </si>
+  <si>
+    <t>FDA Common Data Model Harmonization (CDMH)</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +303,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -397,6 +409,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -415,8 +430,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,19 +741,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E41"/>
+  <dimension ref="B2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="92.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="92.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -748,489 +769,503 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="16"/>
       <c r="D6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>66</v>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="16"/>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="16"/>
       <c r="D12" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <v>3.2</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>42</v>
-      </c>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="4" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
+    <row r="18" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="11">
         <v>3.1</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="4" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
+      <c r="E20" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="4" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="17">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C30" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="17">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="11">
         <v>2.1</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="4" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="s">
+      <c r="E33" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="4" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="4" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="s">
+      <c r="E36" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C37" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C39" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="4" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B28 B33 B36 B38" numberStoredAsText="1"/>
+    <ignoredError sqref="B29 B34 B37 B39" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1241,7 +1276,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1253,7 +1288,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added row in the table for BRIDG 5.2
</commit_message>
<xml_diff>
--- a/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
+++ b/Documents/Graphics/BRIDG Harmonized Project History for use in presentations.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shastak\Documents\Documents\MyDocs\Samvit\Contracts\Attain\BRIDG 5.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shastak\Documents\Documents\MyDocs\Samvit\Contracts\Attain\BRIDG 5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="21984" windowHeight="9972"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
   <si>
     <t>Release</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>FDA Common Data Model Harmonization (CDMH)</t>
+  </si>
+  <si>
+    <t>Aug. 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCI, HL7 </t>
+  </si>
+  <si>
+    <t>IHE Anatomic Pathology Structured Report (APSR) Harmonization, HL7 Specimen DAM Harmonization and BRIDG 5.1 Ballot Comment Resolutions</t>
   </si>
 </sst>
 </file>
@@ -409,33 +418,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E42"/>
+  <dimension ref="B2:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,7 +761,7 @@
     <col min="2" max="2" width="8.5546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="92.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
@@ -769,503 +778,517 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19">
+    <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="12">
+        <v>5.2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D4" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E4" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="16"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>66</v>
+      <c r="B9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="15"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="20">
+        <v>3.2</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="D15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
+    <row r="19" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20">
         <v>3.1</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="4" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
+      <c r="E21" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="4" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="11">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="20">
         <v>2.1</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="4" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
+      <c r="E34" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="4" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="4" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
+      <c r="E37" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C40" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="4" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B29 B34 B37 B39" numberStoredAsText="1"/>
+    <ignoredError sqref="B30 B35 B38 B40" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>